<commit_message>
Merged from origin main
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/data.xlsx
+++ b/src/test/java/TestData/data.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nkosi/Projects/Automation/SauceDemo4thGroup2024/src/test/java/TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ceonline-my.sharepoint.com/personal/thandazani_mbutho_cloudessentials_com/Documents/Personal/Automation Class/SauceDemo4thGroup2024/src/test/java/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A186CB39-79CF-7F43-AE57-B4EC9F5CA88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{A186CB39-79CF-7F43-AE57-B4EC9F5CA88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C3ADB31-584D-4CB6-AE88-A8DE806B4D73}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18980" activeTab="1" xr2:uid="{B8A52318-12D5-3B46-8F7E-8A17FF9AA0D3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{B8A52318-12D5-3B46-8F7E-8A17FF9AA0D3}"/>
   </bookViews>
   <sheets>
     <sheet name="login Details" sheetId="1" r:id="rId1"/>
     <sheet name="User Information" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
   <si>
     <t>Password</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>Cele</t>
+  </si>
+  <si>
+    <t>Tman</t>
+  </si>
+  <si>
+    <t>Mbutho</t>
+  </si>
+  <si>
+    <t>2191</t>
   </si>
 </sst>
 </file>
@@ -159,12 +168,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,13 +515,13 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -519,7 +529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -527,7 +537,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -535,19 +545,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -555,25 +565,25 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -581,18 +591,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="N12" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="N13" s="1" t="s">
@@ -602,7 +612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="L14" t="s">
@@ -615,7 +625,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="N15" s="1" t="s">
@@ -625,7 +635,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="N16" s="1" t="s">
         <v>7</v>
       </c>
@@ -633,7 +643,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="14:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="17" spans="14:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="N17" s="1" t="s">
         <v>8</v>
       </c>
@@ -644,7 +654,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="14:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="18" spans="14:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="O18" s="1" t="s">
         <v>4</v>
       </c>
@@ -652,22 +662,22 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="14:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="19" spans="14:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="O19" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="14:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="20" spans="14:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="O20" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="14:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="21" spans="14:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="O21" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="14:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="22" spans="14:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="O22" s="1" t="s">
         <v>8</v>
       </c>
@@ -682,12 +692,12 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -698,7 +708,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -709,52 +719,58 @@
         <v>2094</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>

</xml_diff>

<commit_message>
Added three methods to capture address details
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/data.xlsx
+++ b/src/test/java/TestData/data.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28122"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nkosi/Projects/Automation/SauceDemo4thGroup2024/src/test/java/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A186CB39-79CF-7F43-AE57-B4EC9F5CA88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{A186CB39-79CF-7F43-AE57-B4EC9F5CA88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A6C754B-2277-4316-9F40-C6D1E2ADDBA5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18980" activeTab="1" xr2:uid="{B8A52318-12D5-3B46-8F7E-8A17FF9AA0D3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18980" firstSheet="1" activeTab="1" xr2:uid="{B8A52318-12D5-3B46-8F7E-8A17FF9AA0D3}"/>
   </bookViews>
   <sheets>
     <sheet name="login Details" sheetId="1" r:id="rId1"/>
     <sheet name="User Information" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
+  <si>
+    <t>username</t>
+  </si>
   <si>
     <t>Password</t>
   </si>
@@ -45,36 +48,33 @@
     <t>standard_user</t>
   </si>
   <si>
-    <t>username</t>
-  </si>
-  <si>
     <t>secret_sauce</t>
   </si>
   <si>
+    <t>problem_user</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>error_user</t>
+  </si>
+  <si>
+    <t>Nkosi</t>
+  </si>
+  <si>
+    <t>visual_user</t>
+  </si>
+  <si>
     <t>locked_out_user</t>
   </si>
   <si>
-    <t>problem_user</t>
+    <t>ß</t>
   </si>
   <si>
     <t>performance_glitch_user</t>
   </si>
   <si>
-    <t>error_user</t>
-  </si>
-  <si>
-    <t>visual_user</t>
-  </si>
-  <si>
-    <t>ß</t>
-  </si>
-  <si>
-    <t>Nkosi</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
     <t>First Name</t>
   </si>
   <si>
@@ -85,13 +85,25 @@
   </si>
   <si>
     <t>Cele</t>
+  </si>
+  <si>
+    <t>2094</t>
+  </si>
+  <si>
+    <t>Simo</t>
+  </si>
+  <si>
+    <t>Mkhasibe</t>
+  </si>
+  <si>
+    <t>2000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -159,12 +171,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,79 +514,79 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F91CAA-A90D-D149-ACA3-285AEDFF15C5}">
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17">
       <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -581,93 +594,93 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="18">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="N12" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="18">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="N13" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="18">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="L14" t="s">
+        <v>10</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:17" ht="18">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="N15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="18">
+      <c r="N16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q15" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="18" x14ac:dyDescent="0.2">
-      <c r="N16" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="Q16" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="14:17" ht="18" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="14:17" ht="18">
       <c r="N17" s="1" t="s">
         <v>8</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="14:17" ht="18" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="14:17" ht="18">
       <c r="O18" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="Q18" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="14:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="19" spans="14:17" ht="18">
       <c r="O19" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="14:17" ht="18" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="14:17" ht="18">
       <c r="O20" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="14:17" ht="18">
+      <c r="O21" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="14:17" ht="18" x14ac:dyDescent="0.2">
-      <c r="O21" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="14:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="22" spans="14:17" ht="18">
       <c r="O22" s="1" t="s">
         <v>8</v>
       </c>
@@ -682,12 +695,12 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -698,63 +711,69 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3">
-        <v>2094</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C2" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>

</xml_diff>

<commit_message>
End to end Testing of Sauce Demo
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/data.xlsx
+++ b/src/test/java/TestData/data.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nkosi/Projects/Automation/SauceDemo4thGroup2024/src/test/java/TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\IdeaProjects\SauceDemo4thGroup2024\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A186CB39-79CF-7F43-AE57-B4EC9F5CA88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18980" activeTab="1" xr2:uid="{B8A52318-12D5-3B46-8F7E-8A17FF9AA0D3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18980" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="login Details" sheetId="1" r:id="rId1"/>
     <sheet name="User Information" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
   <si>
     <t>Password</t>
   </si>
@@ -85,13 +84,16 @@
   </si>
   <si>
     <t>Cele</t>
+  </si>
+  <si>
+    <t>2094</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -159,12 +161,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,20 +501,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F91CAA-A90D-D149-ACA3-285AEDFF15C5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -519,7 +522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -527,7 +530,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -535,19 +538,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -555,25 +558,25 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -581,18 +584,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="17.5">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="N12" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" ht="17.5">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="N13" s="1" t="s">
@@ -602,7 +605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="17.5">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="L14" t="s">
@@ -615,7 +618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" ht="17.5">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="N15" s="1" t="s">
@@ -625,7 +628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" ht="17.5">
       <c r="N16" s="1" t="s">
         <v>7</v>
       </c>
@@ -633,7 +636,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="14:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="17" spans="14:17" ht="17.5">
       <c r="N17" s="1" t="s">
         <v>8</v>
       </c>
@@ -644,7 +647,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="14:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="18" spans="14:17" ht="17.5">
       <c r="O18" s="1" t="s">
         <v>4</v>
       </c>
@@ -652,22 +655,22 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="14:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="19" spans="14:17" ht="17.5">
       <c r="O19" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="14:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="20" spans="14:17" ht="17.5">
       <c r="O20" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="14:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="21" spans="14:17" ht="17.5">
       <c r="O21" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="14:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="22" spans="14:17" ht="17.5">
       <c r="O22" s="1" t="s">
         <v>8</v>
       </c>
@@ -678,16 +681,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22BE7122-9342-A246-9248-C54A3ADB7945}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15.5"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -698,68 +701,69 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3">
-        <v>2094</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C2" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Full test run from login to order completion
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/data.xlsx
+++ b/src/test/java/TestData/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ceonline-my.sharepoint.com/personal/thandazani_mbutho_cloudessentials_com/Documents/Personal/Automation Class/SauceDemo4thGroup2024/src/test/java/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{A186CB39-79CF-7F43-AE57-B4EC9F5CA88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C3ADB31-584D-4CB6-AE88-A8DE806B4D73}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{A186CB39-79CF-7F43-AE57-B4EC9F5CA88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E135BACC-F80D-43E1-A578-37CC7D9777E9}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{B8A52318-12D5-3B46-8F7E-8A17FF9AA0D3}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
   <si>
     <t>Password</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>2191</t>
+  </si>
+  <si>
+    <t>2094</t>
   </si>
 </sst>
 </file>
@@ -692,7 +695,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -715,8 +718,8 @@
       <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3">
-        <v>2094</v>
+      <c r="C2" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>